<commit_message>
dua bai tap len
</commit_message>
<xml_diff>
--- a/DANH MUC BAI TAP.xlsx
+++ b/DANH MUC BAI TAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_CODE_GYM_MY_STUDY\c0523g1_nguyen_thanh_viet_module1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2732FC0-E6EC-4029-8EDD-FC771F0329D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC112C32-F953-45CB-97F2-8503C35E1FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{0C70BF92-38C4-4A6C-B924-8C6078304EB2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s03_pseudocode_flowchart/exercise/%5BB%C3%A0i%20t%E1%BA%ADp%5D%20M%C3%B4%20t%E1%BA%A3%20thu%E1%BA%ADt%20to%C3%A1n%20t%C3%ADnh%20%C4%91i%E1%BB%83m%20trung%20b%C3%ACnh.jpg</t>
   </si>
@@ -104,6 +104,120 @@
   </si>
   <si>
     <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%5D%20T%C3%ADnh%20ch%E1%BB%89%20s%E1%BB%91%20c%C3%A2n%20n%E1%BA%B7ng%20c%E1%BB%A7a%20c%C6%A1%20th%E1%BB%83.html</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 1</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 2</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 3</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 4</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 5</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 6</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 01 - Bài 7</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 1</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 2</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 3</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 4</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 5</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 6</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 7</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 8</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 9</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 10</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 11</t>
+  </si>
+  <si>
+    <t>Luyện tập cấu trúc điều kiện 02 - Bài 12</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-1%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-2%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-3%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-4%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-5%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-6%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-7%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2001.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-8%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-9%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-10%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-11%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-12%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-13%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-14%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-15%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-16%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-19%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-18%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s09_dieu_kien_2/%5BB%C3%A0i%20t%E1%BA%ADp%209-17%5D%20Luy%E1%BB%87n%20t%E1%BA%ADp%20c%E1%BA%A5u%20tr%C3%BAc%20%C4%91i%E1%BB%81u%20ki%E1%BB%87n%2002.html</t>
   </si>
 </sst>
 </file>
@@ -455,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67AC6B5-FAE4-48DF-9576-83A1DC03DDF7}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -562,6 +676,158 @@
         <v>23</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
dua len bai tap
</commit_message>
<xml_diff>
--- a/DANH MUC BAI TAP.xlsx
+++ b/DANH MUC BAI TAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_CODE_GYM_MY_STUDY\c0523g1_nguyen_thanh_viet_module1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15035506-D0F5-4FCA-ACA6-E2A500BCD6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D927F5-EB52-4896-8512-3FC7FE914B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{0C70BF92-38C4-4A6C-B924-8C6078304EB2}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s03_pseudocode_flowchart/exercise/%5BB%C3%A0i%20t%E1%BA%ADp%5D%20M%C3%B4%20t%E1%BA%A3%20thu%E1%BA%ADt%20to%C3%A1n%20t%C3%ADnh%20%C4%91i%E1%BB%83m%20trung%20b%C3%ACnh.jpg</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>[Bài tập] Hiển thị các số nguyên tố đầu tiên</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s11_vong%20lap%202/%5BB%C3%A0i%20t%E1%BA%ADp%5D%20Sinh%20b%E1%BA%A3ng%20c%E1%BB%ADu%20ch%C6%B0%C6%A1ng.html</t>
+  </si>
+  <si>
+    <t>https://github.com/thanhviet05x1d/c0523g1_nguyen_thanh_viet_module1/blob/main/s11_vong%20lap%202/%5BB%C3%A0i%20t%E1%BA%ADp%5D%20Hi%E1%BB%83n%20th%E1%BB%8B%20c%C3%A1c%20s%E1%BB%91%20nguy%C3%AAn%20t%E1%BB%91%20%C4%91%E1%BA%A7u%20ti%C3%AAn.html</t>
   </si>
 </sst>
 </file>
@@ -577,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67AC6B5-FAE4-48DF-9576-83A1DC03DDF7}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -838,10 +844,16 @@
       <c r="A37" t="s">
         <v>62</v>
       </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>